<commit_message>
Reformatted caption for conversion to pdf
</commit_message>
<xml_diff>
--- a/plots/Tables_S1-S4.xlsx
+++ b/plots/Tables_S1-S4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B1B0035-3D8B-418F-A16F-F6223F9505D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C7E4D6-4637-4770-A174-90E9B4AF4CE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="76">
   <si>
     <t>Phylum</t>
   </si>
@@ -279,8 +279,11 @@
     </r>
   </si>
   <si>
+    <t>are presented in the "Comparison" column. For example, in the "Low Fat vs. High Fat" comparison, the left treatment is low fat while the right treatment is high fat.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Supplementary Table S3. Significant OTUs identified in SIMPER analysis of female post-treatment samples. These values are displayed in Fig 6A. </t>
+      <t>Supplementary Table S3. Significant OTUs identified in SIMPER analysis of female post-treatment samples.</t>
     </r>
     <r>
       <rPr>
@@ -290,12 +293,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Left/right treatment" refer to the order in which treatments are presented in the "Comparison" column. For example, in the "Low Fat vs. High Fat" comparison, the left treatment is low fat while the right treatment is high fat.</t>
+      <t xml:space="preserve"> These values are displayed in Fig 6A. "Left/right treatment" refer to the order in which treatments</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Supplementary Table S4. Significant OTUs identified in SIMPER analysis of female post-treatment samples. These values are displayed in Fig 6B. </t>
+      <t xml:space="preserve">Supplementary Table S4. Significant OTUs identified in SIMPER analysis of female post-treatment samples. </t>
     </r>
     <r>
       <rPr>
@@ -305,7 +308,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Left/right treatment" refer to the order in which treatments are presented in the "Comparison" column. For example, in the "Low Fat vs. High Fat" comparison, the left treatment is low fat while the right treatment is high fat.</t>
+      <t>These values are displayed in Fig 6B. "Left/right treatment" refer to the order in which treatments</t>
     </r>
   </si>
 </sst>
@@ -390,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -412,15 +415,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,7 +802,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
@@ -833,7 +837,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -866,7 +870,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -899,7 +903,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -932,7 +936,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="s">
@@ -967,7 +971,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1004,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1033,7 +1037,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1066,7 +1070,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -1099,7 +1103,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1134,7 +1138,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -1167,7 +1171,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1204,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+      <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -1233,7 +1237,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+      <c r="A17" s="19"/>
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -1266,7 +1270,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1299,7 +1303,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B19" t="s">
@@ -1334,7 +1338,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -1367,7 +1371,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -1400,7 +1404,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -1433,7 +1437,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -1466,7 +1470,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
       <c r="B24" t="s">
         <v>21</v>
       </c>
@@ -1499,7 +1503,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
@@ -1607,7 +1611,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
@@ -1642,7 +1646,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -1675,7 +1679,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1708,7 +1712,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1743,7 +1747,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
+      <c r="A8" s="19"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1776,7 +1780,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1809,7 +1813,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1846,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -1875,7 +1879,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1908,7 +1912,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1943,7 +1947,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -1976,7 +1980,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -2009,7 +2013,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
+      <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -2042,7 +2046,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -2075,7 +2079,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2110,7 +2114,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -2143,7 +2147,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -2176,7 +2180,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -2209,7 +2213,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -2242,7 +2246,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
@@ -2287,752 +2291,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D43414C-56A0-4A3F-BF62-2971BE13220F}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2.2587650837568503</v>
-      </c>
-      <c r="I4" s="2">
-        <v>8.6174786187592201</v>
-      </c>
-      <c r="J4" s="2">
-        <v>4.0376811826757004</v>
-      </c>
-      <c r="K4" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1.11865304059293</v>
-      </c>
-      <c r="I5" s="2">
-        <v>9.4726587086459695</v>
-      </c>
-      <c r="J5" s="2">
-        <v>5.3097840253240998</v>
-      </c>
-      <c r="K5" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2">
-        <v>6.5655198307219704</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.52541102433618103</v>
-      </c>
-      <c r="J6" s="2">
-        <v>3.8246076503861999</v>
-      </c>
-      <c r="K6" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="2">
-        <v>6.0981075950843495</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>3.866499920816</v>
-      </c>
-      <c r="K7" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.80865848981640409</v>
-      </c>
-      <c r="I8" s="2">
-        <v>7.1704597439553899</v>
-      </c>
-      <c r="J8" s="2">
-        <v>4.0400235648976999</v>
-      </c>
-      <c r="K8" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.36729856659138704</v>
-      </c>
-      <c r="I9" s="2">
-        <v>7.9580351924304811</v>
-      </c>
-      <c r="J9" s="2">
-        <v>4.8204375287562007</v>
-      </c>
-      <c r="K9" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>6.0722046932876399</v>
-      </c>
-      <c r="J10" s="6">
-        <v>3.8545000100881999</v>
-      </c>
-      <c r="K10" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.36900369003690003</v>
-      </c>
-      <c r="I11" s="4">
-        <v>23.234030814405298</v>
-      </c>
-      <c r="J11" s="2">
-        <v>14.180366809730799</v>
-      </c>
-      <c r="K11" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="2">
-        <v>6.5655198307219704</v>
-      </c>
-      <c r="I12" s="2">
-        <v>6.3169039295412899E-2</v>
-      </c>
-      <c r="J12" s="2">
-        <v>4.0087302405551997</v>
-      </c>
-      <c r="K12" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="2">
-        <v>6.0981075950843495</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>3.7638302977207001</v>
-      </c>
-      <c r="K13" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.36729856659138704</v>
-      </c>
-      <c r="I14" s="2">
-        <v>7.4685918278241505</v>
-      </c>
-      <c r="J14" s="6">
-        <v>4.4044392893957003</v>
-      </c>
-      <c r="K14" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0.36900369003690003</v>
-      </c>
-      <c r="I15" s="4">
-        <v>7.1457036680569503</v>
-      </c>
-      <c r="J15" s="2">
-        <v>4.2215451191964997</v>
-      </c>
-      <c r="K15" s="11">
-        <v>9.7643781073787003E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1.11865304059293</v>
-      </c>
-      <c r="I16" s="2">
-        <v>9.1608022826903799</v>
-      </c>
-      <c r="J16" s="2">
-        <v>4.9780003322138997</v>
-      </c>
-      <c r="K16" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="2">
-        <v>6.5655198307219704</v>
-      </c>
-      <c r="I17" s="2">
-        <v>5.2556237217036207E-2</v>
-      </c>
-      <c r="J17" s="2">
-        <v>4.0150403747942001</v>
-      </c>
-      <c r="K17" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="2">
-        <v>6.0981075950843495</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1.3075313807531401E-2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>3.7554732346579001</v>
-      </c>
-      <c r="K18" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.80865848981640409</v>
-      </c>
-      <c r="I19" s="2">
-        <v>8.6736176747840599</v>
-      </c>
-      <c r="J19" s="2">
-        <v>4.8669892640830001</v>
-      </c>
-      <c r="K19" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.36729856659138704</v>
-      </c>
-      <c r="I20" s="2">
-        <v>8.9152637154191812</v>
-      </c>
-      <c r="J20" s="2">
-        <v>5.2915760377836101</v>
-      </c>
-      <c r="K20" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="6">
-        <v>0</v>
-      </c>
-      <c r="I21" s="6">
-        <v>8.3209335089379604</v>
-      </c>
-      <c r="J21" s="6">
-        <v>5.1480584215701999</v>
-      </c>
-      <c r="K21" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="4">
-        <v>23.234030814405298</v>
-      </c>
-      <c r="I22" s="4">
-        <v>7.1457036680569503</v>
-      </c>
-      <c r="J22" s="2">
-        <v>18.851494311074298</v>
-      </c>
-      <c r="K22" s="11">
-        <v>6.94391649132894E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="6">
-        <v>3.0762450389456899</v>
-      </c>
-      <c r="I23" s="6">
-        <v>8.3209335089379604</v>
-      </c>
-      <c r="J23" s="6">
-        <v>6.0440724423423999</v>
-      </c>
-      <c r="K23" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A23"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6937A552-ED76-4CBC-B641-9B55A9C9C2BB}">
-  <dimension ref="A1:K21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3055,113 +2318,835 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.2587650837568503</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8.6174786187592201</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4.0376811826757004</v>
+      </c>
+      <c r="K5" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.11865304059293</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9.4726587086459695</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.3097840253240998</v>
+      </c>
+      <c r="K6" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6.5655198307219704</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.52541102433618103</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3.8246076503861999</v>
+      </c>
+      <c r="K7" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2">
+        <v>6.0981075950843495</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3.866499920816</v>
+      </c>
+      <c r="K8" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.80865848981640409</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7.1704597439553899</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.0400235648976999</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.36729856659138704</v>
+      </c>
+      <c r="I10" s="2">
+        <v>7.9580351924304811</v>
+      </c>
+      <c r="J10" s="2">
+        <v>4.8204375287562007</v>
+      </c>
+      <c r="K10" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>6.0722046932876399</v>
+      </c>
+      <c r="J11" s="6">
+        <v>3.8545000100881999</v>
+      </c>
+      <c r="K11" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.36900369003690003</v>
+      </c>
+      <c r="I12" s="4">
+        <v>23.234030814405298</v>
+      </c>
+      <c r="J12" s="2">
+        <v>14.180366809730799</v>
+      </c>
+      <c r="K12" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="2">
+        <v>6.5655198307219704</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.3169039295412899E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>4.0087302405551997</v>
+      </c>
+      <c r="K13" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2">
+        <v>6.0981075950843495</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3.7638302977207001</v>
+      </c>
+      <c r="K14" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.36729856659138704</v>
+      </c>
+      <c r="I15" s="2">
+        <v>7.4685918278241505</v>
+      </c>
+      <c r="J15" s="6">
+        <v>4.4044392893957003</v>
+      </c>
+      <c r="K15" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.36900369003690003</v>
+      </c>
+      <c r="I16" s="4">
+        <v>7.1457036680569503</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4.2215451191964997</v>
+      </c>
+      <c r="K16" s="11">
+        <v>9.7643781073787003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.11865304059293</v>
+      </c>
+      <c r="I17" s="2">
+        <v>9.1608022826903799</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.9780003322138997</v>
+      </c>
+      <c r="K17" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2">
+        <v>6.5655198307219704</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5.2556237217036207E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4.0150403747942001</v>
+      </c>
+      <c r="K18" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="2">
+        <v>6.0981075950843495</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.3075313807531401E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3.7554732346579001</v>
+      </c>
+      <c r="K19" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.80865848981640409</v>
+      </c>
+      <c r="I20" s="2">
+        <v>8.6736176747840599</v>
+      </c>
+      <c r="J20" s="2">
+        <v>4.8669892640830001</v>
+      </c>
+      <c r="K20" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.36729856659138704</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8.9152637154191812</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.2915760377836101</v>
+      </c>
+      <c r="K21" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
+        <v>8.3209335089379604</v>
+      </c>
+      <c r="J22" s="6">
+        <v>5.1480584215701999</v>
+      </c>
+      <c r="K22" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="4">
+        <v>23.234030814405298</v>
+      </c>
+      <c r="I23" s="4">
+        <v>7.1457036680569503</v>
+      </c>
+      <c r="J23" s="2">
+        <v>18.851494311074298</v>
+      </c>
+      <c r="K23" s="11">
+        <v>6.94391649132894E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="6">
+        <v>3.0762450389456899</v>
+      </c>
+      <c r="I24" s="6">
+        <v>8.3209335089379604</v>
+      </c>
+      <c r="J24" s="6">
+        <v>6.0440724423423999</v>
+      </c>
+      <c r="K24" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6937A552-ED76-4CBC-B641-9B55A9C9C2BB}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="22"/>
+    </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="4">
         <v>1.3201606728158999</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I5" s="4">
         <v>11.207461724708899</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J5" s="4">
         <v>6.14293675148605</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K5" s="13">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.81422532288610794</v>
-      </c>
-      <c r="I5" s="2">
-        <v>5.1182388324432804</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2.6742865111275003</v>
-      </c>
-      <c r="K5" s="11">
-        <v>6.02462820456654E-2</v>
-      </c>
-    </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -3172,363 +3157,363 @@
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
+        <v>70</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2">
-        <v>0.366877543479392</v>
+        <v>0.81422532288610794</v>
       </c>
       <c r="I6" s="2">
-        <v>7.2520780107844098</v>
+        <v>5.1182388324432804</v>
       </c>
       <c r="J6" s="2">
-        <v>4.2826943254382996</v>
+        <v>2.6742865111275003</v>
       </c>
       <c r="K6" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>0.366877543479392</v>
       </c>
       <c r="I7" s="2">
-        <v>6.74449079184323</v>
+        <v>7.2520780107844098</v>
       </c>
       <c r="J7" s="2">
-        <v>4.1972979779216999</v>
+        <v>4.2826943254382996</v>
       </c>
       <c r="K7" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6.74449079184323</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4.1972979779216999</v>
+      </c>
+      <c r="K8" s="11">
+        <v>6.02462820456654E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H9" s="6">
         <v>4.2171108857500101</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I9" s="6">
         <v>0.21010210446763999</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J9" s="6">
         <v>2.5122404073045002</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K9" s="12">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H10" s="4">
         <v>1.0378827192527201E-2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I10" s="4">
         <v>5.4548799587369894</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J10" s="4">
         <v>3.4897901747986002</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K10" s="13">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>40</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <v>1.3201606728158999</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <v>10.288825821618699</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J11" s="2">
         <v>5.7419035410682007</v>
-      </c>
-      <c r="K10" s="11">
-        <v>6.02462820456654E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.81422532288610794</v>
-      </c>
-      <c r="I11" s="2">
-        <v>8.2825433876669301</v>
-      </c>
-      <c r="J11" s="2">
-        <v>4.7804209387312007</v>
       </c>
       <c r="K11" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>0.81422532288610794</v>
       </c>
       <c r="I12" s="2">
-        <v>3.3154936871767502</v>
+        <v>8.2825433876669301</v>
       </c>
       <c r="J12" s="2">
-        <v>2.1232660071107001</v>
+        <v>4.7804209387312007</v>
       </c>
       <c r="K12" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3.3154936871767502</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2.1232660071107001</v>
+      </c>
+      <c r="K13" s="11">
+        <v>6.02462820456654E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H14" s="6">
         <v>4.2171108857500101</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I14" s="6">
         <v>0.31480485177355699</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J14" s="6">
         <v>2.5241393916153001</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K14" s="12">
         <v>9.9256213736009694E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H15" s="4">
         <v>1.0378827192527201E-2</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I15" s="4">
         <v>6.9279110647711306</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J15" s="4">
         <v>4.3441527534359006</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K15" s="13">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="19"/>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>40</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <v>1.3201606728158999</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <v>8.4008939738959487</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
         <v>4.4426768456995998</v>
-      </c>
-      <c r="K15" s="11">
-        <v>6.02462820456654E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.81422532288610794</v>
-      </c>
-      <c r="I16" s="2">
-        <v>6.6625249054209998</v>
-      </c>
-      <c r="J16" s="2">
-        <v>3.6772556540592998</v>
       </c>
       <c r="K16" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+      <c r="A17" s="19"/>
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -3539,62 +3524,62 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
+        <v>70</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H17" s="2">
-        <v>0.366877543479392</v>
+        <v>0.81422532288610794</v>
       </c>
       <c r="I17" s="2">
-        <v>6.6216937334744594</v>
+        <v>6.6625249054209998</v>
       </c>
       <c r="J17" s="2">
-        <v>3.9317200600686997</v>
+        <v>3.6772556540592998</v>
       </c>
       <c r="K17" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
+      <c r="A18" s="19"/>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>0.366877543479392</v>
       </c>
       <c r="I18" s="2">
-        <v>9.0916493002914898</v>
+        <v>6.6216937334744594</v>
       </c>
       <c r="J18" s="2">
-        <v>5.7166997033284401</v>
+        <v>3.9317200600686997</v>
       </c>
       <c r="K18" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -3605,100 +3590,133 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="H19" s="2">
-        <v>5.2221526311168505E-2</v>
+        <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>6.9894092464400606</v>
+        <v>9.0916493002914898</v>
       </c>
       <c r="J19" s="2">
-        <v>4.3576714804441998</v>
+        <v>5.7166997033284401</v>
       </c>
       <c r="K19" s="11">
         <v>6.02462820456654E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.2221526311168505E-2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>6.9894092464400606</v>
+      </c>
+      <c r="J20" s="2">
+        <v>4.3576714804441998</v>
+      </c>
+      <c r="K20" s="11">
+        <v>6.02462820456654E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H21" s="6">
         <v>4.2171108857500101</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I21" s="6">
         <v>0.27559428012645498</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J21" s="6">
         <v>2.4977565447616001</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K21" s="12">
         <v>7.9019822908659595E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="15" t="s">
+      <c r="B22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E22" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F22" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H22" s="17">
         <v>3.3154936871767502</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I22" s="17">
         <v>9.0916493002914898</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J22" s="17">
         <v>6.7658064513314002</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K22" s="18">
         <v>7.9993340997447607E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Relabeled tables to include mean rel abund in legend
</commit_message>
<xml_diff>
--- a/plots/Tables_S1-S4.xlsx
+++ b/plots/Tables_S1-S4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C7E4D6-4637-4770-A174-90E9B4AF4CE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C028D7-6B0D-43E5-BA29-DB61E0430E07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="2" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Variation Explained (%)</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>OTU</t>
   </si>
   <si>
@@ -247,6 +244,24 @@
   </si>
   <si>
     <t>Ruminicoccaceae</t>
+  </si>
+  <si>
+    <t>are presented in the "Comparison" column. For example, in the "Low Fat vs. High Fat" comparison, the left treatment is low fat while the right treatment is high fat.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Supplementary Table S4. Significant OTUs identified in SIMPER analysis of female post-treatment samples. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>These mean relative abundances are displayed in Fig 6B. "Left/right treatment" refer to the order in which treatments</t>
+    </r>
   </si>
   <si>
     <r>
@@ -260,7 +275,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>These values are displayed in Supplementary Figure S1A.</t>
+      <t>These mean relative abundances are displayed in Supplementary Figure S1A.</t>
     </r>
   </si>
   <si>
@@ -275,11 +290,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> These values are displayed in Supplementary Figure S1B.</t>
+      <t xml:space="preserve"> These mean relative abundances are displayed in Supplementary Figure S1B.</t>
     </r>
-  </si>
-  <si>
-    <t>are presented in the "Comparison" column. For example, in the "Low Fat vs. High Fat" comparison, the left treatment is low fat while the right treatment is high fat.</t>
   </si>
   <si>
     <r>
@@ -293,23 +305,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> These values are displayed in Fig 6A. "Left/right treatment" refer to the order in which treatments</t>
+      <t xml:space="preserve"> These mean relative abundances are displayed in Fig 6A. "Left/right treatment" refer to the order in which treatments</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Supplementary Table S4. Significant OTUs identified in SIMPER analysis of female post-treatment samples. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>These values are displayed in Fig 6B. "Left/right treatment" refer to the order in which treatments</t>
-    </r>
+    <t>Adjusted P</t>
   </si>
 </sst>
 </file>
@@ -415,6 +415,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,7 +425,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF5B042-A855-4564-AE29-BF999DFF7221}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -760,7 +762,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -768,7 +770,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -786,42 +788,42 @@
         <v>4</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>49</v>
+      <c r="A4" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="2">
         <v>1.8315018315018299</v>
@@ -837,24 +839,24 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2">
         <v>7.6143586699441004</v>
@@ -870,24 +872,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2">
         <v>5.1547022912672498</v>
@@ -903,24 +905,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="6">
         <v>0.12585212375458799</v>
@@ -936,26 +938,26 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>50</v>
+      <c r="A8" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2">
         <v>16.121661713962098</v>
@@ -971,24 +973,24 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2">
         <v>6.7811573550801096</v>
@@ -1004,24 +1006,24 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="2">
         <v>0.73877263513410008</v>
@@ -1037,24 +1039,24 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="2">
         <v>11.3454541365053</v>
@@ -1070,24 +1072,24 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" s="2">
         <v>2.6385224274406299E-2</v>
@@ -1103,26 +1105,26 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>51</v>
+      <c r="A13" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" s="4">
         <v>4.95662102094317</v>
@@ -1138,24 +1140,24 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H14" s="2">
         <v>11.3949021461075</v>
@@ -1171,24 +1173,24 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H15" s="2">
         <v>1.9</v>
@@ -1204,24 +1206,24 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="2">
         <v>7.0863145067829896</v>
@@ -1237,24 +1239,24 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
@@ -1270,24 +1272,24 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="6">
         <v>5.2478470978697196</v>
@@ -1303,26 +1305,26 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
-        <v>52</v>
+      <c r="A19" s="20" t="s">
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" s="2">
         <v>13.0002360802747</v>
@@ -1338,24 +1340,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20" s="2">
         <v>10.300042701471099</v>
@@ -1371,24 +1373,24 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" s="2">
         <v>1.3330412191829901</v>
@@ -1404,24 +1406,24 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" s="2">
         <v>6.9195026164312097</v>
@@ -1437,24 +1439,24 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
@@ -1470,24 +1472,24 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -1503,24 +1505,24 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H25" s="6">
         <v>6.6078719039071006</v>
@@ -1550,7 +1552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B06FDC-51D2-4D6E-AEB1-1C7CC06C82DD}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1569,7 +1573,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1577,7 +1581,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -1595,42 +1599,42 @@
         <v>4</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>49</v>
+      <c r="A4" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="2">
         <v>9.7327087865713793</v>
@@ -1646,24 +1650,24 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="2">
         <v>9.8167708623264289</v>
@@ -1679,24 +1683,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="6">
         <v>8.3953027338985103E-2</v>
@@ -1712,26 +1716,26 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>50</v>
+      <c r="A7" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="4">
         <v>1.0422094841063099E-2</v>
@@ -1747,24 +1751,24 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8" s="2">
         <v>5.1426305450752503</v>
@@ -1780,24 +1784,24 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2">
         <v>10.586231890697901</v>
@@ -1813,24 +1817,24 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="2">
         <v>1.1356231577854001</v>
@@ -1846,24 +1850,24 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="2">
         <v>0.43107626342188704</v>
@@ -1879,24 +1883,24 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="6">
         <v>0</v>
@@ -1912,26 +1916,26 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>51</v>
+      <c r="A13" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" s="4">
         <v>7.3325516264755901</v>
@@ -1947,24 +1951,24 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="2">
         <v>4.9845278161482502</v>
@@ -1980,24 +1984,24 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2">
         <v>20.9121728325742</v>
@@ -2013,24 +2017,24 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="2">
         <v>1.9242604322280401</v>
@@ -2046,24 +2050,24 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="6">
         <v>0</v>
@@ -2079,26 +2083,26 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
-        <v>52</v>
+      <c r="A18" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="4">
         <v>11.740558033632199</v>
@@ -2114,24 +2118,24 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="2">
         <v>1.0803608991414799</v>
@@ -2147,24 +2151,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="2">
         <v>0.38145014404241301</v>
@@ -2180,24 +2184,24 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21" s="2">
         <v>14.0181294244826</v>
@@ -2213,24 +2217,24 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -2246,24 +2250,24 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H23" s="6">
         <v>5.3107466569911894E-2</v>
@@ -2294,7 +2298,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2318,8 +2322,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>73</v>
+      <c r="A2" s="19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2327,7 +2331,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -2345,42 +2349,42 @@
         <v>4</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>67</v>
+      <c r="A5" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="2">
         <v>2.2587650837568503</v>
@@ -2396,24 +2400,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="2">
         <v>1.11865304059293</v>
@@ -2429,24 +2433,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2">
         <v>6.5655198307219704</v>
@@ -2462,24 +2466,24 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2">
         <v>6.0981075950843495</v>
@@ -2495,24 +2499,24 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="2">
         <v>0.80865848981640409</v>
@@ -2528,24 +2532,24 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="2">
         <v>0.36729856659138704</v>
@@ -2561,24 +2565,24 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6">
         <v>0</v>
@@ -2594,26 +2598,26 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>68</v>
+      <c r="A12" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" s="4">
         <v>0.36900369003690003</v>
@@ -2629,24 +2633,24 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2">
         <v>6.5655198307219704</v>
@@ -2662,24 +2666,24 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="2">
         <v>6.0981075950843495</v>
@@ -2695,24 +2699,24 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="2">
         <v>0.36729856659138704</v>
@@ -2728,26 +2732,26 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>69</v>
+      <c r="A16" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" s="4">
         <v>0.36900369003690003</v>
@@ -2763,24 +2767,24 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="2">
         <v>1.11865304059293</v>
@@ -2796,24 +2800,24 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" s="2">
         <v>6.5655198307219704</v>
@@ -2829,24 +2833,24 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2">
         <v>6.0981075950843495</v>
@@ -2862,24 +2866,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="2">
         <v>0.80865848981640409</v>
@@ -2895,24 +2899,24 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="2">
         <v>0.36729856659138704</v>
@@ -2928,24 +2932,24 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="6">
         <v>0</v>
@@ -2961,26 +2965,26 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
-        <v>66</v>
+      <c r="A23" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" s="4">
         <v>23.234030814405298</v>
@@ -2996,24 +3000,24 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" s="6">
         <v>3.0762450389456899</v>
@@ -3044,7 +3048,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3064,20 +3068,20 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>73</v>
+      <c r="A2" s="19" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
+      <c r="A3" s="19"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -3095,42 +3099,42 @@
         <v>4</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>67</v>
+      <c r="A5" s="22" t="s">
+        <v>66</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="4">
         <v>1.3201606728158999</v>
@@ -3146,24 +3150,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="2">
         <v>0.81422532288610794</v>
@@ -3179,24 +3183,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2">
         <v>0.366877543479392</v>
@@ -3212,24 +3216,24 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -3245,24 +3249,24 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="6">
         <v>4.2171108857500101</v>
@@ -3278,26 +3282,26 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>68</v>
+      <c r="A10" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" s="4">
         <v>1.0378827192527201E-2</v>
@@ -3313,24 +3317,24 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="2">
         <v>1.3201606728158999</v>
@@ -3346,24 +3350,24 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="2">
         <v>0.81422532288610794</v>
@@ -3379,24 +3383,24 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -3412,24 +3416,24 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="6">
         <v>4.2171108857500101</v>
@@ -3445,26 +3449,26 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>69</v>
+      <c r="A15" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" s="4">
         <v>1.0378827192527201E-2</v>
@@ -3480,24 +3484,24 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="2">
         <v>1.3201606728158999</v>
@@ -3513,24 +3517,24 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="2">
         <v>0.81422532288610794</v>
@@ -3546,24 +3550,24 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="2">
         <v>0.366877543479392</v>
@@ -3579,24 +3583,24 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
@@ -3612,24 +3616,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H20" s="2">
         <v>5.2221526311168505E-2</v>
@@ -3645,24 +3649,24 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" s="6">
         <v>4.2171108857500101</v>
@@ -3679,25 +3683,25 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="17">
         <v>3.3154936871767502</v>

</xml_diff>

<commit_message>
Fixed Table S4 caption label (males, not females)
</commit_message>
<xml_diff>
--- a/plots/Tables_S1-S4.xlsx
+++ b/plots/Tables_S1-S4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C028D7-6B0D-43E5-BA29-DB61E0430E07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3817C23E-8A18-4B6F-A49F-D4288A58A14A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="2" r:id="rId1"/>
@@ -250,21 +250,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Supplementary Table S4. Significant OTUs identified in SIMPER analysis of female post-treatment samples. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>These mean relative abundances are displayed in Fig 6B. "Left/right treatment" refer to the order in which treatments</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Supplementary Table S1. Significant OTUs identified in SIMPER analysis of female pre- versus post-treatment. </t>
     </r>
     <r>
@@ -310,6 +295,21 @@
   </si>
   <si>
     <t>Adjusted P</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Supplementary Table S4. Significant OTUs identified in SIMPER analysis of male post-treatment samples. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>These mean relative abundances are displayed in Fig 6B. "Left/right treatment" refer to the order in which treatments</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -762,7 +762,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -800,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1573,7 +1573,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1611,7 +1611,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2296,756 +2296,6 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D43414C-56A0-4A3F-BF62-2971BE13220F}">
   <dimension ref="A1:K24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2.2587650837568503</v>
-      </c>
-      <c r="I5" s="2">
-        <v>8.6174786187592201</v>
-      </c>
-      <c r="J5" s="2">
-        <v>4.0376811826757004</v>
-      </c>
-      <c r="K5" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.11865304059293</v>
-      </c>
-      <c r="I6" s="2">
-        <v>9.4726587086459695</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5.3097840253240998</v>
-      </c>
-      <c r="K6" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2">
-        <v>6.5655198307219704</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.52541102433618103</v>
-      </c>
-      <c r="J7" s="2">
-        <v>3.8246076503861999</v>
-      </c>
-      <c r="K7" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="2">
-        <v>6.0981075950843495</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>3.866499920816</v>
-      </c>
-      <c r="K8" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.80865848981640409</v>
-      </c>
-      <c r="I9" s="2">
-        <v>7.1704597439553899</v>
-      </c>
-      <c r="J9" s="2">
-        <v>4.0400235648976999</v>
-      </c>
-      <c r="K9" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.36729856659138704</v>
-      </c>
-      <c r="I10" s="2">
-        <v>7.9580351924304811</v>
-      </c>
-      <c r="J10" s="2">
-        <v>4.8204375287562007</v>
-      </c>
-      <c r="K10" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>6.0722046932876399</v>
-      </c>
-      <c r="J11" s="6">
-        <v>3.8545000100881999</v>
-      </c>
-      <c r="K11" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.36900369003690003</v>
-      </c>
-      <c r="I12" s="4">
-        <v>23.234030814405298</v>
-      </c>
-      <c r="J12" s="2">
-        <v>14.180366809730799</v>
-      </c>
-      <c r="K12" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="2">
-        <v>6.5655198307219704</v>
-      </c>
-      <c r="I13" s="2">
-        <v>6.3169039295412899E-2</v>
-      </c>
-      <c r="J13" s="2">
-        <v>4.0087302405551997</v>
-      </c>
-      <c r="K13" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="2">
-        <v>6.0981075950843495</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>3.7638302977207001</v>
-      </c>
-      <c r="K14" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.36729856659138704</v>
-      </c>
-      <c r="I15" s="2">
-        <v>7.4685918278241505</v>
-      </c>
-      <c r="J15" s="6">
-        <v>4.4044392893957003</v>
-      </c>
-      <c r="K15" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0.36900369003690003</v>
-      </c>
-      <c r="I16" s="4">
-        <v>7.1457036680569503</v>
-      </c>
-      <c r="J16" s="2">
-        <v>4.2215451191964997</v>
-      </c>
-      <c r="K16" s="11">
-        <v>9.7643781073787003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1.11865304059293</v>
-      </c>
-      <c r="I17" s="2">
-        <v>9.1608022826903799</v>
-      </c>
-      <c r="J17" s="2">
-        <v>4.9780003322138997</v>
-      </c>
-      <c r="K17" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2">
-        <v>6.5655198307219704</v>
-      </c>
-      <c r="I18" s="2">
-        <v>5.2556237217036207E-2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>4.0150403747942001</v>
-      </c>
-      <c r="K18" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="2">
-        <v>6.0981075950843495</v>
-      </c>
-      <c r="I19" s="2">
-        <v>1.3075313807531401E-2</v>
-      </c>
-      <c r="J19" s="2">
-        <v>3.7554732346579001</v>
-      </c>
-      <c r="K19" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.80865848981640409</v>
-      </c>
-      <c r="I20" s="2">
-        <v>8.6736176747840599</v>
-      </c>
-      <c r="J20" s="2">
-        <v>4.8669892640830001</v>
-      </c>
-      <c r="K20" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.36729856659138704</v>
-      </c>
-      <c r="I21" s="2">
-        <v>8.9152637154191812</v>
-      </c>
-      <c r="J21" s="2">
-        <v>5.2915760377836101</v>
-      </c>
-      <c r="K21" s="11">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6">
-        <v>8.3209335089379604</v>
-      </c>
-      <c r="J22" s="6">
-        <v>5.1480584215701999</v>
-      </c>
-      <c r="K22" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="4">
-        <v>23.234030814405298</v>
-      </c>
-      <c r="I23" s="4">
-        <v>7.1457036680569503</v>
-      </c>
-      <c r="J23" s="2">
-        <v>18.851494311074298</v>
-      </c>
-      <c r="K23" s="11">
-        <v>6.94391649132894E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="6">
-        <v>3.0762450389456899</v>
-      </c>
-      <c r="I24" s="6">
-        <v>8.3209335089379604</v>
-      </c>
-      <c r="J24" s="6">
-        <v>6.0440724423423999</v>
-      </c>
-      <c r="K24" s="12">
-        <v>3.8149009161145699E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A23:A24"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6937A552-ED76-4CBC-B641-9B55A9C9C2BB}">
-  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
@@ -3068,7 +2318,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3077,7 +2327,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -3111,7 +2361,757 @@
         <v>5</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.2587650837568503</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8.6174786187592201</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4.0376811826757004</v>
+      </c>
+      <c r="K5" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.11865304059293</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9.4726587086459695</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.3097840253240998</v>
+      </c>
+      <c r="K6" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6.5655198307219704</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.52541102433618103</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3.8246076503861999</v>
+      </c>
+      <c r="K7" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <v>6.0981075950843495</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3.866499920816</v>
+      </c>
+      <c r="K8" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.80865848981640409</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7.1704597439553899</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.0400235648976999</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.36729856659138704</v>
+      </c>
+      <c r="I10" s="2">
+        <v>7.9580351924304811</v>
+      </c>
+      <c r="J10" s="2">
+        <v>4.8204375287562007</v>
+      </c>
+      <c r="K10" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>6.0722046932876399</v>
+      </c>
+      <c r="J11" s="6">
+        <v>3.8545000100881999</v>
+      </c>
+      <c r="K11" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.36900369003690003</v>
+      </c>
+      <c r="I12" s="4">
+        <v>23.234030814405298</v>
+      </c>
+      <c r="J12" s="2">
+        <v>14.180366809730799</v>
+      </c>
+      <c r="K12" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2">
+        <v>6.5655198307219704</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.3169039295412899E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>4.0087302405551997</v>
+      </c>
+      <c r="K13" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2">
+        <v>6.0981075950843495</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3.7638302977207001</v>
+      </c>
+      <c r="K14" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.36729856659138704</v>
+      </c>
+      <c r="I15" s="2">
+        <v>7.4685918278241505</v>
+      </c>
+      <c r="J15" s="6">
+        <v>4.4044392893957003</v>
+      </c>
+      <c r="K15" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.36900369003690003</v>
+      </c>
+      <c r="I16" s="4">
+        <v>7.1457036680569503</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4.2215451191964997</v>
+      </c>
+      <c r="K16" s="11">
+        <v>9.7643781073787003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.11865304059293</v>
+      </c>
+      <c r="I17" s="2">
+        <v>9.1608022826903799</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.9780003322138997</v>
+      </c>
+      <c r="K17" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2">
+        <v>6.5655198307219704</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5.2556237217036207E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4.0150403747942001</v>
+      </c>
+      <c r="K18" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2">
+        <v>6.0981075950843495</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.3075313807531401E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3.7554732346579001</v>
+      </c>
+      <c r="K19" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.80865848981640409</v>
+      </c>
+      <c r="I20" s="2">
+        <v>8.6736176747840599</v>
+      </c>
+      <c r="J20" s="2">
+        <v>4.8669892640830001</v>
+      </c>
+      <c r="K20" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.36729856659138704</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8.9152637154191812</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.2915760377836101</v>
+      </c>
+      <c r="K21" s="11">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
+        <v>8.3209335089379604</v>
+      </c>
+      <c r="J22" s="6">
+        <v>5.1480584215701999</v>
+      </c>
+      <c r="K22" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="4">
+        <v>23.234030814405298</v>
+      </c>
+      <c r="I23" s="4">
+        <v>7.1457036680569503</v>
+      </c>
+      <c r="J23" s="2">
+        <v>18.851494311074298</v>
+      </c>
+      <c r="K23" s="11">
+        <v>6.94391649132894E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="6">
+        <v>3.0762450389456899</v>
+      </c>
+      <c r="I24" s="6">
+        <v>8.3209335089379604</v>
+      </c>
+      <c r="J24" s="6">
+        <v>6.0440724423423999</v>
+      </c>
+      <c r="K24" s="12">
+        <v>3.8149009161145699E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6937A552-ED76-4CBC-B641-9B55A9C9C2BB}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made PDFs of all figs/tables
</commit_message>
<xml_diff>
--- a/plots/Tables_S1-S4.xlsx
+++ b/plots/Tables_S1-S4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3817C23E-8A18-4B6F-A49F-D4288A58A14A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC95BDEA-CCD8-4EFC-B8F1-434CD85631C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79FB6064-B257-4C80-A5A4-F82625E9D2A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Table S3" sheetId="4" r:id="rId3"/>
     <sheet name="Table S4" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Table S3'!$A$1:$K$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -741,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF5B042-A855-4564-AE29-BF999DFF7221}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1545,6 +1548,7 @@
     <mergeCell ref="A19:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2290,6 +2294,7 @@
     <mergeCell ref="A18:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2297,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D43414C-56A0-4A3F-BF62-2971BE13220F}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3040,6 +3045,7 @@
     <mergeCell ref="A23:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3723,5 +3729,6 @@
     <mergeCell ref="A15:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>